<commit_message>
Interkation und HMI zur Aufgabenvorstellung hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumente/Notizen/2_StandDerTechnik/Tabelle-Assistenzsysteme(HMI).xlsx
+++ b/Dokumente/Notizen/2_StandDerTechnik/Tabelle-Assistenzsysteme(HMI).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meret/Documents/Uni/TU_Dresden/Diplomarbeit/Dokumente/Notizen/2_StandDerTechnik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meret Feldkamper\Documents\Diplomarbeit\Diplomarbeit\Dokumente\Notizen\2_StandDerTechnik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E177D52-AEA2-0F4D-998E-D1E074510BDD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Assistenz" sheetId="1" r:id="rId1"/>
@@ -541,7 +540,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -793,61 +792,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1129,27 +1128,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5" style="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1172,11 +1171,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1190,9 +1189,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="19"/>
+    <row r="3" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1206,9 +1205,9 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="19"/>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1221,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="16" t="s">
         <v>85</v>
@@ -1246,7 +1245,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
         <v>102</v>
@@ -1266,7 +1265,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="16"/>
       <c r="C7" s="3"/>
@@ -1280,7 +1279,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="10"/>
       <c r="C8" s="3"/>
@@ -1294,11 +1293,11 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1318,9 +1317,9 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="19"/>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1336,9 +1335,9 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="19"/>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
@@ -1352,9 +1351,9 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="19"/>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
@@ -1368,9 +1367,9 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1394,9 +1393,9 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="19"/>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1418,9 +1417,9 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="19"/>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
@@ -1438,7 +1437,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="16" t="s">
         <v>85</v>
@@ -1458,7 +1457,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="16" t="s">
         <v>102</v>
@@ -1474,7 +1473,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="16" t="s">
         <v>156</v>
@@ -1492,7 +1491,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="16"/>
       <c r="C19" s="3" t="s">
@@ -1508,7 +1507,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1521,11 +1520,11 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1549,9 +1548,9 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="19"/>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="3" t="s">
         <v>38</v>
       </c>
@@ -1573,9 +1572,9 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="19"/>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
@@ -1591,8 +1590,8 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1607,11 +1606,11 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1635,9 +1634,9 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="19"/>
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
@@ -1659,9 +1658,9 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
-      <c r="B27" s="19"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>55</v>
@@ -1677,8 +1676,8 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
@@ -1693,8 +1692,8 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
@@ -1704,11 +1703,11 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -1727,9 +1726,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="19"/>
+    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
@@ -1744,9 +1743,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
-      <c r="B32" s="19"/>
+    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="3" t="s">
         <v>69</v>
       </c>
@@ -1755,9 +1754,9 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
-      <c r="B33" s="24" t="s">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -1776,9 +1775,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="19"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>97</v>
@@ -1793,9 +1792,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="19"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1804,8 +1803,8 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
       <c r="B36" s="9"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1813,8 +1812,8 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="28" t="s">
@@ -1836,8 +1835,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
       <c r="B38" s="29"/>
       <c r="C38" s="15" t="s">
         <v>78</v>
@@ -1855,8 +1854,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
       <c r="B39" s="29"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
@@ -1868,8 +1867,8 @@
       </c>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="33"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14" t="s">
@@ -1881,7 +1880,7 @@
       </c>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>101</v>
       </c>
@@ -1894,7 +1893,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1903,7 +1902,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1912,7 +1911,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1921,7 +1920,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1930,7 +1929,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1939,16 +1938,11 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="33"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B25:B27"/>
@@ -1958,6 +1952,11 @@
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1965,27 +1964,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97D2128-2023-1748-AE6C-056027C4F791}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.5" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="35.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -2004,11 +2003,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -2024,9 +2023,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
-      <c r="B3" s="19"/>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15" t="s">
         <v>109</v>
       </c>
@@ -2038,8 +2037,8 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
       <c r="B4" s="16" t="s">
         <v>159</v>
       </c>
@@ -2052,11 +2051,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C5" s="6"/>
@@ -2064,10 +2063,10 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>159</v>
       </c>
@@ -2078,10 +2077,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>164</v>
       </c>
@@ -2099,15 +2098,15 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C12" s="6"/>
@@ -2119,15 +2118,15 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -2137,25 +2136,25 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-    </row>
-    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -2171,8 +2170,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B20" s="19"/>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
       <c r="C20" s="3" t="s">
         <v>124</v>
       </c>
@@ -2180,8 +2179,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="22"/>
       <c r="C21" s="3" t="s">
         <v>130</v>
       </c>
@@ -2189,8 +2188,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="19"/>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
       <c r="C22" s="3" t="s">
         <v>132</v>
       </c>
@@ -2198,14 +2197,14 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B23" s="19"/>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
       <c r="C23" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
+    <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="34"/>
       <c r="C24" s="3" t="s">
         <v>135</v>
       </c>
@@ -2213,11 +2212,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -2233,8 +2232,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B26" s="19"/>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
       <c r="C26" s="3" t="s">
         <v>139</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>143</v>
       </c>
@@ -2253,12 +2252,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>106</v>
       </c>
@@ -2266,11 +2265,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -2283,8 +2282,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="B31" s="19"/>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="22"/>
       <c r="E31" s="3" t="s">
         <v>151</v>
       </c>
@@ -2292,12 +2291,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="E32" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="5:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" ht="30" x14ac:dyDescent="0.25">
       <c r="E33" s="3" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Tabellen zum Thema Assistenz hinzugefügt (Latex)
</commit_message>
<xml_diff>
--- a/Dokumente/Notizen/2_StandDerTechnik/Tabelle-Assistenzsysteme(HMI).xlsx
+++ b/Dokumente/Notizen/2_StandDerTechnik/Tabelle-Assistenzsysteme(HMI).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meret Feldkamper\Documents\Diplomarbeit\Diplomarbeit\Dokumente\Notizen\2_StandDerTechnik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meret/Documents/Uni/TU_Dresden/Diplomarbeit/Dokumente/Notizen/2_StandDerTechnik/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD670D3-09FA-A746-BD81-93E82ADF83D5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assistenz" sheetId="1" r:id="rId1"/>
@@ -168,9 +169,6 @@
     <t>Beschäftigung muss unterbrochen werden</t>
   </si>
   <si>
-    <t>Konzentration auf Handeheld und ursprüngliche Aufgabe gleichzeitig</t>
-  </si>
-  <si>
     <t>Unterarmcomputer</t>
   </si>
   <si>
@@ -535,12 +533,15 @@
   </si>
   <si>
     <t>Eingabe mittls Berührung</t>
+  </si>
+  <si>
+    <t>Pr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -807,37 +808,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1128,27 +1129,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="29.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1171,8 +1172,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -1189,8 +1190,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+    <row r="3" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="33"/>
       <c r="B3" s="22"/>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -1205,8 +1206,8 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
       <c r="B4" s="22"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -1221,23 +1222,23 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1245,18 +1246,18 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="3"/>
@@ -1265,7 +1266,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="16"/>
       <c r="C7" s="3"/>
@@ -1279,7 +1280,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="10"/>
       <c r="C8" s="3"/>
@@ -1293,8 +1294,8 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -1317,8 +1318,8 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
       <c r="B10" s="22"/>
       <c r="C10" s="3" t="s">
         <v>15</v>
@@ -1335,8 +1336,8 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
       <c r="B11" s="22"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1351,8 +1352,8 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
       <c r="B12" s="22"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1367,9 +1368,9 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27" t="s">
+    <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1393,8 +1394,8 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
       <c r="B14" s="22"/>
       <c r="C14" s="3" t="s">
         <v>23</v>
@@ -1417,8 +1418,8 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
       <c r="B15" s="22"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1437,18 +1438,18 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1457,10 +1458,10 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1473,13 +1474,13 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1491,11 +1492,11 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="16"/>
       <c r="C19" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1507,7 +1508,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1520,8 +1521,8 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -1548,8 +1549,8 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
       <c r="B22" s="22"/>
       <c r="C22" s="3" t="s">
         <v>38</v>
@@ -1572,8 +1573,8 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
       <c r="B23" s="22"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1590,13 +1591,13 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1606,27 +1607,27 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>48</v>
+    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="F25" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1634,20 +1635,20 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
       <c r="B26" s="22"/>
       <c r="C26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>34</v>
@@ -1658,15 +1659,15 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
       <c r="B27" s="22"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1676,12 +1677,12 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1692,119 +1693,119 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
+    <row r="29" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>62</v>
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="F30" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
       <c r="B31" s="22"/>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
       <c r="B32" s="22"/>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27" t="s">
+    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="F33" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
       <c r="B34" s="22"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="24"/>
       <c r="B35" s="22"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
+    <row r="36" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
       <c r="B36" s="9"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1812,80 +1813,80 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="30"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F37" s="13" t="s">
+      <c r="E38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="29"/>
+    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="30"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="33"/>
+    <row r="40" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1893,7 +1894,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1902,7 +1903,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1911,7 +1912,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1920,7 +1921,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1929,7 +1930,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1938,11 +1939,16 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B25:B27"/>
@@ -1952,11 +1958,6 @@
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1964,26 +1965,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="3"/>
+    <col min="1" max="1" width="35.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2000,305 +2001,305 @@
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
       <c r="B3" s="22"/>
       <c r="C3" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>123</v>
-      </c>
       <c r="B19" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" s="22"/>
       <c r="C20" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="B21" s="22"/>
       <c r="C21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="22"/>
       <c r="C22" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="22"/>
       <c r="C23" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="34"/>
       <c r="C24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>138</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="22"/>
       <c r="C26" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="D27" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D28" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E27" s="3" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="F30" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="B31" s="22"/>
       <c r="E31" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="E32" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E32" s="3" t="s">
+    </row>
+    <row r="33" spans="5:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="E33" s="3" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="E33" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>